<commit_message>
Add semester 7 unified timetable with baskets (9 AM-5:30 PM, 2 classes per basket)
</commit_message>
<xml_diff>
--- a/sdtt_inputs/classroom_data.xlsx
+++ b/sdtt_inputs/classroom_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saini\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/55835114c1b5d5ed/Desktop/tt.1/sdtt_inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B590D3A7-9DA7-42D6-A7F6-1E539B57CFDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{B590D3A7-9DA7-42D6-A7F6-1E539B57CFDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A8B7022-67DF-43C6-9091-4E2A9AB82240}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{44EF9099-EFE8-424E-A0F9-69DBDE7FAFFD}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
   <si>
     <r>
       <rPr>
@@ -94,16 +92,6 @@
         <rFont val="Calibri"/>
         <family val="1"/>
       </rPr>
-      <t>Recreation</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
       <t>nil</t>
     </r>
   </si>
@@ -636,6 +624,9 @@
       </rPr>
       <t>L408</t>
     </r>
+  </si>
+  <si>
+    <t>large classroom</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1020,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1059,367 +1050,367 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="2">
+        <v>120</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="3">
+        <v>120</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="3">
-        <v>116</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3">
         <v>135</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="29">
       <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C5" s="3">
         <v>240</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3">
         <v>96</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3">
         <v>96</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3">
         <v>96</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C10" s="3">
         <v>40</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C11" s="3">
         <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="3">
         <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="3">
         <v>96</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="3">
         <v>96</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="3">
         <v>96</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="3">
         <v>96</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="3">
         <v>40</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="3">
         <v>40</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="3">
         <v>40</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="3">
         <v>96</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" s="3">
         <v>96</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="3">
         <v>96</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="3">
         <v>96</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="3">
         <v>96</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C28" s="3">
         <v>40</v>
@@ -1428,10 +1419,10 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="3">
         <v>40</v>
@@ -1440,112 +1431,112 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31" s="3">
         <v>80</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C32" s="3">
         <v>80</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C33" s="3">
         <v>80</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C34" s="3">
         <v>80</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C35" s="3">
         <v>80</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C36" s="3">
         <v>80</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C37" s="3">
         <v>80</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>